<commit_message>
#1245 PMD Rule 위반 수정 (천정호)
 미사용 변수 제거 및 수정 
 ToDoList_Main.java
</commit_message>
<xml_diff>
--- a/Subject_Dir/Subject_List.xlsx
+++ b/Subject_Dir/Subject_List.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="21">
   <si>
     <t>과목</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>2-4</t>
   </si>
 </sst>
 </file>

</xml_diff>